<commit_message>
list admin -- this workflow is terrible
</commit_message>
<xml_diff>
--- a/BR_Mailer/J020_DS_FSC_BR/J020_Mailing_List - Excel.xlsx
+++ b/BR_Mailer/J020_DS_FSC_BR/J020_Mailing_List - Excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Business Reporting\zDev\BR_Scripts\BRPoSh\BR_Mailer\J020_DS_FSC_BR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Business Reporting\ZDEV\BR_Scripts\BRPoSh\BR_Mailer\J020_DS_FSC_BR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -204,55 +204,55 @@
     <t>Jacquie.Russo@henryschein.ca,Jason.Brown@henryschein.ca,Jason.Schuler@henryschein.com,Marc.Zdrojewski@henryschein.com</t>
   </si>
   <si>
-    <t>201711_ATLTC_FSCBook.pdf</t>
-  </si>
-  <si>
-    <t>201711_CALGY_FSCBook.pdf</t>
-  </si>
-  <si>
-    <t>201711_EDMON_FSCBook.pdf</t>
-  </si>
-  <si>
-    <t>201711_LONDN_FSCBook.pdf</t>
-  </si>
-  <si>
-    <t>201711_MEDIC_FSCBook.pdf</t>
-  </si>
-  <si>
-    <t>201711_MNTRL_FSCBook.pdf</t>
-  </si>
-  <si>
-    <t>201711_NWFLD_FSCBook.pdf</t>
-  </si>
-  <si>
-    <t>201711_OTTWA_FSCBook.pdf</t>
-  </si>
-  <si>
-    <t>201711_PRAIR_FSCBook.pdf</t>
-  </si>
-  <si>
-    <t>201711_QUEBC_FSCBook.pdf</t>
-  </si>
-  <si>
-    <t>201711_TORNT1_FSCBook.pdf</t>
-  </si>
-  <si>
-    <t>201711_TORNT2_FSCBook.pdf</t>
-  </si>
-  <si>
-    <t>201711_TORNT3_FSCBook.pdf</t>
-  </si>
-  <si>
-    <t>201711_TORNT4_FSCBook.pdf</t>
-  </si>
-  <si>
-    <t>201711_TORNT5_FSCBook.pdf</t>
-  </si>
-  <si>
-    <t>201711_VACVR_FSCBook.pdf</t>
-  </si>
-  <si>
-    <t>201711_VICTR_FSCBook.pdf</t>
+    <t>201712_ATLTC_FSCBook.pdf</t>
+  </si>
+  <si>
+    <t>201712_CALGY_FSCBook.pdf</t>
+  </si>
+  <si>
+    <t>201712_EDMON_FSCBook.pdf</t>
+  </si>
+  <si>
+    <t>201712_LONDN_FSCBook.pdf</t>
+  </si>
+  <si>
+    <t>201712_MEDIC_FSCBook.pdf</t>
+  </si>
+  <si>
+    <t>201712_MNTRL_FSCBook.pdf</t>
+  </si>
+  <si>
+    <t>201712_NWFLD_FSCBook.pdf</t>
+  </si>
+  <si>
+    <t>201712_OTTWA_FSCBook.pdf</t>
+  </si>
+  <si>
+    <t>201712_PRAIR_FSCBook.pdf</t>
+  </si>
+  <si>
+    <t>201712_QUEBC_FSCBook.pdf</t>
+  </si>
+  <si>
+    <t>201712_TORNT1_FSCBook.pdf</t>
+  </si>
+  <si>
+    <t>201712_TORNT2_FSCBook.pdf</t>
+  </si>
+  <si>
+    <t>201712_TORNT3_FSCBook.pdf</t>
+  </si>
+  <si>
+    <t>201712_TORNT4_FSCBook.pdf</t>
+  </si>
+  <si>
+    <t>201712_TORNT5_FSCBook.pdf</t>
+  </si>
+  <si>
+    <t>201712_VACVR_FSCBook.pdf</t>
+  </si>
+  <si>
+    <t>201712_VICTR_FSCBook.pdf</t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -680,14 +682,14 @@
       </c>
       <c r="G2" t="str">
         <f>$K2&amp;"\"&amp;L2</f>
-        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201711_ATLTC_FSCBook.pdf</v>
+        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201712_ATLTC_FSCBook.pdf</v>
       </c>
       <c r="K2" t="s">
         <v>59</v>
       </c>
       <c r="L2" t="str">
         <f>L3</f>
-        <v>201711_ATLTC_FSCBook.pdf</v>
+        <v>201712_ATLTC_FSCBook.pdf</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -711,7 +713,7 @@
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3" si="0">$K3&amp;"\"&amp;L3</f>
-        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201711_ATLTC_FSCBook.pdf</v>
+        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201712_ATLTC_FSCBook.pdf</v>
       </c>
       <c r="K3" t="s">
         <v>59</v>
@@ -741,7 +743,7 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" ref="G4:G17" si="1">$K4&amp;"\"&amp;L4</f>
-        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201711_CALGY_FSCBook.pdf</v>
+        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201712_CALGY_FSCBook.pdf</v>
       </c>
       <c r="K4" t="s">
         <v>59</v>
@@ -771,7 +773,7 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="1"/>
-        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201711_EDMON_FSCBook.pdf</v>
+        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201712_EDMON_FSCBook.pdf</v>
       </c>
       <c r="K5" t="s">
         <v>59</v>
@@ -801,7 +803,7 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="1"/>
-        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201711_LONDN_FSCBook.pdf</v>
+        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201712_LONDN_FSCBook.pdf</v>
       </c>
       <c r="K6" t="s">
         <v>59</v>
@@ -831,7 +833,7 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
-        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201711_MEDIC_FSCBook.pdf</v>
+        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201712_MEDIC_FSCBook.pdf</v>
       </c>
       <c r="K7" t="s">
         <v>59</v>
@@ -861,7 +863,7 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
-        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201711_MNTRL_FSCBook.pdf</v>
+        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201712_MNTRL_FSCBook.pdf</v>
       </c>
       <c r="K8" t="s">
         <v>59</v>
@@ -891,7 +893,7 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
-        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201711_NWFLD_FSCBook.pdf</v>
+        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201712_NWFLD_FSCBook.pdf</v>
       </c>
       <c r="K9" t="s">
         <v>59</v>
@@ -921,7 +923,7 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
-        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201711_OTTWA_FSCBook.pdf</v>
+        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201712_OTTWA_FSCBook.pdf</v>
       </c>
       <c r="K10" t="s">
         <v>59</v>
@@ -951,7 +953,7 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
-        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201711_PRAIR_FSCBook.pdf</v>
+        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201712_PRAIR_FSCBook.pdf</v>
       </c>
       <c r="K11" t="s">
         <v>59</v>
@@ -981,7 +983,7 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="1"/>
-        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201711_QUEBC_FSCBook.pdf</v>
+        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201712_QUEBC_FSCBook.pdf</v>
       </c>
       <c r="K12" t="s">
         <v>59</v>
@@ -1011,7 +1013,7 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" si="1"/>
-        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201711_TORNT1_FSCBook.pdf</v>
+        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201712_TORNT1_FSCBook.pdf</v>
       </c>
       <c r="K13" t="s">
         <v>59</v>
@@ -1041,7 +1043,7 @@
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
-        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201711_TORNT2_FSCBook.pdf</v>
+        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201712_TORNT2_FSCBook.pdf</v>
       </c>
       <c r="K14" t="s">
         <v>59</v>
@@ -1071,7 +1073,7 @@
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
-        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201711_TORNT3_FSCBook.pdf</v>
+        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201712_TORNT3_FSCBook.pdf</v>
       </c>
       <c r="K15" t="s">
         <v>59</v>
@@ -1101,7 +1103,7 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
-        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201711_TORNT4_FSCBook.pdf</v>
+        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201712_TORNT4_FSCBook.pdf</v>
       </c>
       <c r="K16" t="s">
         <v>59</v>
@@ -1131,7 +1133,7 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="1"/>
-        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201711_TORNT5_FSCBook.pdf</v>
+        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201712_TORNT5_FSCBook.pdf</v>
       </c>
       <c r="K17" t="s">
         <v>59</v>
@@ -1161,7 +1163,7 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" ref="G18:G19" si="2">$K18&amp;"\"&amp;L18</f>
-        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201711_VACVR_FSCBook.pdf</v>
+        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201712_VACVR_FSCBook.pdf</v>
       </c>
       <c r="K18" t="s">
         <v>59</v>
@@ -1191,7 +1193,7 @@
       </c>
       <c r="G19" t="str">
         <f t="shared" si="2"/>
-        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201711_VICTR_FSCBook.pdf</v>
+        <v>S:\Business Reporting\RegularReports\Weekly\Weekly FSC Reports\Send\201712_VICTR_FSCBook.pdf</v>
       </c>
       <c r="K19" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
PO Acrual + maint
</commit_message>
<xml_diff>
--- a/BR_Mailer/J020_DS_FSC_BR/J020_Mailing_List - Excel.xlsx
+++ b/BR_Mailer/J020_DS_FSC_BR/J020_Mailing_List - Excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Business Reporting\ZDEV\BR_Scripts\BRPoSh\BR_Mailer\J020_DS_FSC_BR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Business Reporting\zDev\BR_Scripts\BRPoSh\BR_Mailer\J020_DS_FSC_BR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -201,9 +201,6 @@
     <t>Christian.Marsolais@henryschein.ca,Frederic.Gagnon@henryschein.ca,Jacquie.Russo@henryschein.ca</t>
   </si>
   <si>
-    <t>Alain.Maranda@henryschein.ca,Christian.Marsolais@henryschein.ca,Jacquie.Russo@henryschein.ca,Jean-Francois.Carmichael@henryschein.ca</t>
-  </si>
-  <si>
     <t>201802_ATLTC_FSCBook.pdf</t>
   </si>
   <si>
@@ -253,6 +250,9 @@
   </si>
   <si>
     <t>201802_VICTR_FSCBook.pdf</t>
+  </si>
+  <si>
+    <t>Christian.Marsolais@henryschein.ca,Jacquie.Russo@henryschein.ca,Jean-Francois.Carmichael@henryschein.ca</t>
   </si>
 </sst>
 </file>
@@ -615,7 +615,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -728,7 +730,7 @@
         <v>53</v>
       </c>
       <c r="L3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -758,7 +760,7 @@
         <v>53</v>
       </c>
       <c r="L4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -788,7 +790,7 @@
         <v>53</v>
       </c>
       <c r="L5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -818,7 +820,7 @@
         <v>53</v>
       </c>
       <c r="L6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -848,7 +850,7 @@
         <v>53</v>
       </c>
       <c r="L7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -878,7 +880,7 @@
         <v>53</v>
       </c>
       <c r="L8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -908,7 +910,7 @@
         <v>53</v>
       </c>
       <c r="L9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -938,7 +940,7 @@
         <v>53</v>
       </c>
       <c r="L10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -968,7 +970,7 @@
         <v>53</v>
       </c>
       <c r="L11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -976,7 +978,7 @@
         <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
         <v>50</v>
@@ -998,7 +1000,7 @@
         <v>53</v>
       </c>
       <c r="L12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1028,7 +1030,7 @@
         <v>53</v>
       </c>
       <c r="L13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1058,7 +1060,7 @@
         <v>53</v>
       </c>
       <c r="L14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1088,7 +1090,7 @@
         <v>53</v>
       </c>
       <c r="L15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1118,7 +1120,7 @@
         <v>53</v>
       </c>
       <c r="L16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1148,7 +1150,7 @@
         <v>53</v>
       </c>
       <c r="L17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1178,7 +1180,7 @@
         <v>53</v>
       </c>
       <c r="L18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1208,7 +1210,7 @@
         <v>53</v>
       </c>
       <c r="L19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>